<commit_message>
Thêm khung Controller BNS
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/account.xlsx
+++ b/Hethongquanlylab/wwwroot/data/account.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB17970-C879-41D3-B933-A1651578B4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A90CE4-E173-4A85-9A2D-A49089008D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>UserName</t>
   </si>
@@ -40,14 +40,19 @@
   </si>
   <si>
     <t>user</t>
+  </si>
+  <si>
+    <t>BanNhanSu</t>
+  </si>
+  <si>
+    <t>super</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,7 +79,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
@@ -358,82 +363,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
         <v>40001</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="0">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3">
         <v>40002</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>40002</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="0">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
         <v>50001</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>50001</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="0">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5">
         <v>50002</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>50002</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="0">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6">
         <v>50003</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>50003</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>12345</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Thêm giao diện Ban Đào tạo
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/account.xlsx
+++ b/Hethongquanlylab/wwwroot/data/account.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Hethongquanly\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A90CE4-E173-4A85-9A2D-A49089008D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F32537D-5748-4DD0-9FBA-E79500DCDF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>UserName</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>super</t>
+  </si>
+  <si>
+    <t>BanDaoTao</t>
   </si>
 </sst>
 </file>
@@ -82,7 +85,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,15 +366,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -382,7 +388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>40001</v>
       </c>
@@ -393,7 +399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>40002</v>
       </c>
@@ -404,7 +410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50001</v>
       </c>
@@ -415,7 +421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50002</v>
       </c>
@@ -426,7 +432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50003</v>
       </c>
@@ -437,7 +443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -445,6 +451,17 @@
         <v>12345</v>
       </c>
       <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>12345</v>
+      </c>
+      <c r="C8" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hoàn thành cơ bản BDH
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/account.xlsx
+++ b/Hethongquanlylab/wwwroot/data/account.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Hethongquanly\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE1F846-AD5C-4C5F-BFC7-BFE5F8842687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352EA5E8-2156-4B2E-8BA3-029CD6283076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16536" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>UserName</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>BanTruyenThong</t>
+  </si>
+  <si>
+    <t>BanDieuHanh</t>
   </si>
 </sst>
 </file>
@@ -372,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,6 +496,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>12345</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Hoàn thiện Super Controller thiếu AddProject, EditProject chưa hoạt động, mới copy code sang PTLT
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/account.xlsx
+++ b/Hethongquanlylab/wwwroot/data/account.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Hethongquanly\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352EA5E8-2156-4B2E-8BA3-029CD6283076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E0DFEA-D289-43BA-970B-010A7B91A101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16536" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8544" yWindow="2736" windowWidth="14496" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>UserName</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>BanDieuHanh</t>
+  </si>
+  <si>
+    <t>PTLT</t>
   </si>
 </sst>
 </file>
@@ -375,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,6 +510,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>12345</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Thêm thành viên Ban/PT Notifications Layout EditNoti, AddNoti NotificationDetail của Home Nút chuyển trang thông báo trang chủ và n thứ lỗi khác :)))))
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/account.xlsx
+++ b/Hethongquanlylab/wwwroot/data/account.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Hethongquanly\Hethongquanlylab\wwwroot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E0DFEA-D289-43BA-970B-010A7B91A101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4373DB1D-607C-4D25-B881-3B2E67928E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8544" yWindow="2736" windowWidth="14496" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>UserName</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>PTLT</t>
+  </si>
+  <si>
+    <t>BanDoiSong</t>
   </si>
 </sst>
 </file>
@@ -378,18 +381,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="14.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,7 +403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>40001</v>
       </c>
@@ -411,7 +414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>40002</v>
       </c>
@@ -422,7 +425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>50001</v>
       </c>
@@ -433,7 +436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>50002</v>
       </c>
@@ -444,7 +447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>50003</v>
       </c>
@@ -455,7 +458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -466,7 +469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -477,7 +480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -488,7 +491,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -499,7 +502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -510,7 +513,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -518,6 +521,17 @@
         <v>12345</v>
       </c>
       <c r="C12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>12345</v>
+      </c>
+      <c r="C13" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Chức năng quản lý biểu mẫu + Quản lý Link
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/account.xlsx
+++ b/Hethongquanlylab/wwwroot/data/account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4373DB1D-607C-4D25-B881-3B2E67928E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA11E45-D6C7-425B-A607-6E31F9499E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>UserName</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>BanDoiSong</t>
+  </si>
+  <si>
+    <t>BanCoVan</t>
   </si>
 </sst>
 </file>
@@ -381,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -535,6 +538,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>12345</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Chức năng quản lý tài khoản
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/account.xlsx
+++ b/Hethongquanlylab/wwwroot/data/account.xlsx
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>UserName</t>
   </si>
@@ -67,13 +67,86 @@
   </si>
   <si>
     <t>BanCoVan</t>
+  </si>
+  <si>
+    <t>001100A2</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>323</t>
+  </si>
+  <si>
+    <t>3221</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>9999</t>
+  </si>
+  <si>
+    <t>99999</t>
+  </si>
+  <si>
+    <t>999213</t>
+  </si>
+  <si>
+    <t>dfg</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>2345</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>5021</t>
+  </si>
+  <si>
+    <t>a9</t>
+  </si>
+  <si>
+    <t>0212</t>
+  </si>
+  <si>
+    <t>0213AA</t>
+  </si>
+  <si>
+    <t>234A</t>
+  </si>
+  <si>
+    <t>A1234</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>ds33</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,10 +173,10 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
@@ -395,161 +468,470 @@
     <col min="1" max="1" width="14.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" s="0">
         <v>40001</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3">
+    <row r="3">
+      <c r="A3" s="0">
         <v>40002</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>40002</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4">
+    <row r="4">
+      <c r="A4" s="0">
         <v>50001</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>50001</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5">
+    <row r="5">
+      <c r="A5" s="0">
         <v>50002</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>50002</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6">
+    <row r="6">
+      <c r="A6" s="0">
         <v>50003</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>50003</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="7">
+      <c r="A7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0">
         <v>12345</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="8">
+      <c r="A8" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <v>12345</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="9">
+      <c r="A9" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <v>12345</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="10">
+      <c r="A10" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0">
         <v>12345</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="11">
+      <c r="A11" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="0">
         <v>12345</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="12">
+      <c r="A12" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="0">
         <v>12345</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="13">
+      <c r="A13" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="0">
         <v>12345</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+    <row r="14">
+      <c r="A14" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="0">
         <v>12345</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="0" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>